<commit_message>
Added handler for Patient Status
</commit_message>
<xml_diff>
--- a/resources/hca_category_codes.xlsx
+++ b/resources/hca_category_codes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otrob\Documents\Dev\HaitiApp\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D072168-86D4-4B6D-8807-132D5573FF0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4239A6-B4D5-4C62-8291-CA2D5D293E37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20480" yWindow="3420" windowWidth="17660" windowHeight="14300" activeTab="8" xr2:uid="{6B3C05BC-D8F6-47BC-A5E5-1D1A72CFB519}"/>
+    <workbookView xWindow="13670" yWindow="860" windowWidth="10220" windowHeight="7060" activeTab="3" xr2:uid="{6B3C05BC-D8F6-47BC-A5E5-1D1A72CFB519}"/>
   </bookViews>
   <sheets>
     <sheet name="ClinicalEncounterType" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -110,18 +110,6 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Pre-Op</t>
-  </si>
-  <si>
-    <t>Awaiting Diagnosis</t>
-  </si>
-  <si>
-    <t>Following Non-Surgically</t>
-  </si>
-  <si>
-    <t>Post-Op</t>
-  </si>
-  <si>
     <t>T21</t>
   </si>
   <si>
@@ -192,6 +180,24 @@
   </si>
   <si>
     <t>Assigned Task</t>
+  </si>
+  <si>
+    <t>1 Preop</t>
+  </si>
+  <si>
+    <t>2 For Exam</t>
+  </si>
+  <si>
+    <t>4 Following</t>
+  </si>
+  <si>
+    <t>5 Post-Op</t>
+  </si>
+  <si>
+    <t>3 No Contact</t>
+  </si>
+  <si>
+    <t>Deceased Preop</t>
   </si>
 </sst>
 </file>
@@ -558,12 +564,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -579,7 +585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -587,7 +593,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -595,7 +601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -616,13 +622,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -644,7 +650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -668,12 +674,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -689,7 +695,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -697,7 +703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -705,7 +711,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -720,18 +726,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C3D5BE-DCDF-4163-B69A-AFB892850139}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -739,36 +745,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -784,13 +806,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,37 +823,37 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -847,13 +869,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -861,7 +883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -869,36 +891,36 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -914,13 +936,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -931,23 +953,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -966,76 +988,76 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1053,17 +1075,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382AA366-6878-4799-BCA0-DB885E605AF8}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1071,31 +1093,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Added urgency and syndrome import handlers to hca.py, corrected category spreadsheet
</commit_message>
<xml_diff>
--- a/resources/hca_category_codes.xlsx
+++ b/resources/hca_category_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otrob\Documents\Dev\HaitiApp\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4239A6-B4D5-4C62-8291-CA2D5D293E37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D09B19-315C-4EFF-BF11-F4F2AD3C55CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13670" yWindow="860" windowWidth="10220" windowHeight="7060" activeTab="3" xr2:uid="{6B3C05BC-D8F6-47BC-A5E5-1D1A72CFB519}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="4" xr2:uid="{6B3C05BC-D8F6-47BC-A5E5-1D1A72CFB519}"/>
   </bookViews>
   <sheets>
     <sheet name="ClinicalEncounterType" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>id</t>
   </si>
@@ -119,27 +119,6 @@
     <t>NS</t>
   </si>
   <si>
-    <t>Down Syndrome</t>
-  </si>
-  <si>
-    <t>Williams Syndrome</t>
-  </si>
-  <si>
-    <t>Noonan Syndrome</t>
-  </si>
-  <si>
-    <t>&lt;6 months</t>
-  </si>
-  <si>
-    <t>6-12 months</t>
-  </si>
-  <si>
-    <t>12-24 months</t>
-  </si>
-  <si>
-    <t>&gt;24 months</t>
-  </si>
-  <si>
     <t>Cardiologist</t>
   </si>
   <si>
@@ -197,7 +176,43 @@
     <t>3 No Contact</t>
   </si>
   <si>
-    <t>Deceased Preop</t>
+    <t>6 Deceased Preop</t>
+  </si>
+  <si>
+    <t>&lt;6 mos</t>
+  </si>
+  <si>
+    <t>6-12 mos</t>
+  </si>
+  <si>
+    <t>12-24 mos</t>
+  </si>
+  <si>
+    <t>&gt;2 years</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>Holt-Oram</t>
+  </si>
+  <si>
+    <t>Marfan</t>
+  </si>
+  <si>
+    <t>Noonan</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>HO</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>OS</t>
   </si>
 </sst>
 </file>
@@ -229,7 +244,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -237,13 +252,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C3D5BE-DCDF-4163-B69A-AFB892850139}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -750,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -758,7 +783,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -766,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -774,7 +799,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -782,7 +807,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -790,7 +815,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -800,10 +825,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52535282-E6A0-43C8-98EF-9D760650685A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,7 +853,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -839,10 +864,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -850,10 +875,43 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -866,7 +924,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -895,32 +953,32 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>28</v>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
+      <c r="B4" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
+      <c r="B5" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>31</v>
+      <c r="B6" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -958,10 +1016,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -969,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -998,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1006,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1014,7 +1072,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1022,7 +1080,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1030,7 +1088,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1038,7 +1096,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1046,7 +1104,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1054,7 +1112,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1098,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1106,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1114,7 +1172,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added passport priority import handler to hca.py
</commit_message>
<xml_diff>
--- a/resources/hca_category_codes.xlsx
+++ b/resources/hca_category_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otrob\Documents\Dev\HaitiApp\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D09B19-315C-4EFF-BF11-F4F2AD3C55CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AE22A5-32CD-40E2-BB87-257E56261D55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="4" xr2:uid="{6B3C05BC-D8F6-47BC-A5E5-1D1A72CFB519}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{6B3C05BC-D8F6-47BC-A5E5-1D1A72CFB519}"/>
   </bookViews>
   <sheets>
     <sheet name="ClinicalEncounterType" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>OS</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -693,10 +696,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF88981-8B50-4F78-9C5B-B8BB3D2D03D2}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,6 +745,14 @@
       </c>
       <c r="B5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -827,7 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52535282-E6A0-43C8-98EF-9D760650685A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added handler for surgical encounter import with placeholders for surgeon, facility, type
</commit_message>
<xml_diff>
--- a/resources/hca_category_codes.xlsx
+++ b/resources/hca_category_codes.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otrob\Documents\Dev\HaitiApp\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AE22A5-32CD-40E2-BB87-257E56261D55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90D5ACB-3683-4FA7-8ED4-D37AD9D7E43F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{6B3C05BC-D8F6-47BC-A5E5-1D1A72CFB519}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" firstSheet="1" activeTab="3" xr2:uid="{6B3C05BC-D8F6-47BC-A5E5-1D1A72CFB519}"/>
   </bookViews>
   <sheets>
     <sheet name="ClinicalEncounterType" sheetId="1" r:id="rId1"/>
     <sheet name="FacilityCategory" sheetId="5" r:id="rId2"/>
     <sheet name="PassportPriority" sheetId="6" r:id="rId3"/>
-    <sheet name="PatientStatus" sheetId="9" r:id="rId4"/>
-    <sheet name="PatientSyndrome" sheetId="7" r:id="rId5"/>
-    <sheet name="PatientUrgency" sheetId="8" r:id="rId6"/>
-    <sheet name="ProviderCategory" sheetId="4" r:id="rId7"/>
-    <sheet name="TravelDocumentDocType" sheetId="2" r:id="rId8"/>
-    <sheet name="TravelDocumentEventType" sheetId="3" r:id="rId9"/>
+    <sheet name="Surgery" sheetId="10" r:id="rId4"/>
+    <sheet name="PatientStatus" sheetId="9" r:id="rId5"/>
+    <sheet name="PatientSyndrome" sheetId="7" r:id="rId6"/>
+    <sheet name="PatientUrgency" sheetId="8" r:id="rId7"/>
+    <sheet name="ProviderCategory" sheetId="4" r:id="rId8"/>
+    <sheet name="TravelDocumentDocType" sheetId="2" r:id="rId9"/>
+    <sheet name="TravelDocumentEventType" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>id</t>
   </si>
@@ -216,6 +217,33 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>surgery_name</t>
+  </si>
+  <si>
+    <t>rachs_score</t>
+  </si>
+  <si>
+    <t>TOF surgery</t>
+  </si>
+  <si>
+    <t>VSD surgery</t>
+  </si>
+  <si>
+    <t>ASD surgery</t>
+  </si>
+  <si>
+    <t>TOF</t>
+  </si>
+  <si>
+    <t>VSD</t>
+  </si>
+  <si>
+    <t>ASD</t>
   </si>
 </sst>
 </file>
@@ -642,6 +670,65 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382AA366-6878-4799-BCA0-DB885E605AF8}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA287ED-1109-45DA-A1EB-69188F036B86}">
   <dimension ref="A1:C3"/>
@@ -698,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF88981-8B50-4F78-9C5B-B8BB3D2D03D2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -761,6 +848,80 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598A50A3-9E4E-4CFB-ADBD-32D4519A3413}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="16.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C3D5BE-DCDF-4163-B69A-AFB892850139}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -834,7 +995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52535282-E6A0-43C8-98EF-9D760650685A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -930,7 +1091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6536046B-55FA-4C27-8C41-A3DB3D50526B}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -997,7 +1158,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244A02C7-843C-4898-AB5D-5B841F681527}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1049,7 +1210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BCE8E8F-D3A3-40F1-8833-268875482DC5}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1138,63 +1299,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382AA366-6878-4799-BCA0-DB885E605AF8}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.1796875" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added fake starter data for providers and facilities
</commit_message>
<xml_diff>
--- a/resources/hca_category_codes.xlsx
+++ b/resources/hca_category_codes.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otrob\Documents\Dev\HaitiApp\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90D5ACB-3683-4FA7-8ED4-D37AD9D7E43F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9B0A21-CF2B-4C60-9464-5254C1F0C939}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" firstSheet="1" activeTab="3" xr2:uid="{6B3C05BC-D8F6-47BC-A5E5-1D1A72CFB519}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{6B3C05BC-D8F6-47BC-A5E5-1D1A72CFB519}"/>
   </bookViews>
   <sheets>
     <sheet name="ClinicalEncounterType" sheetId="1" r:id="rId1"/>
-    <sheet name="FacilityCategory" sheetId="5" r:id="rId2"/>
-    <sheet name="PassportPriority" sheetId="6" r:id="rId3"/>
-    <sheet name="Surgery" sheetId="10" r:id="rId4"/>
-    <sheet name="PatientStatus" sheetId="9" r:id="rId5"/>
-    <sheet name="PatientSyndrome" sheetId="7" r:id="rId6"/>
-    <sheet name="PatientUrgency" sheetId="8" r:id="rId7"/>
-    <sheet name="ProviderCategory" sheetId="4" r:id="rId8"/>
-    <sheet name="TravelDocumentDocType" sheetId="2" r:id="rId9"/>
-    <sheet name="TravelDocumentEventType" sheetId="3" r:id="rId10"/>
+    <sheet name="Provider" sheetId="12" r:id="rId2"/>
+    <sheet name="Facility" sheetId="11" r:id="rId3"/>
+    <sheet name="FacilityCategory" sheetId="5" r:id="rId4"/>
+    <sheet name="PassportPriority" sheetId="6" r:id="rId5"/>
+    <sheet name="Surgery" sheetId="10" r:id="rId6"/>
+    <sheet name="PatientStatus" sheetId="9" r:id="rId7"/>
+    <sheet name="PatientSyndrome" sheetId="7" r:id="rId8"/>
+    <sheet name="PatientUrgency" sheetId="8" r:id="rId9"/>
+    <sheet name="ProviderCategory" sheetId="4" r:id="rId10"/>
+    <sheet name="TravelDocumentDocType" sheetId="2" r:id="rId11"/>
+    <sheet name="TravelDocumentEventType" sheetId="3" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>id</t>
   </si>
@@ -244,6 +246,120 @@
   </si>
   <si>
     <t>ASD</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Hospital A</t>
+  </si>
+  <si>
+    <t>Hospital B</t>
+  </si>
+  <si>
+    <t>Hospital C</t>
+  </si>
+  <si>
+    <t>Clinic A</t>
+  </si>
+  <si>
+    <t>Hospital D</t>
+  </si>
+  <si>
+    <t>Clinic B</t>
+  </si>
+  <si>
+    <t>Clinic C</t>
+  </si>
+  <si>
+    <t>Clinic D</t>
+  </si>
+  <si>
+    <t>note1</t>
+  </si>
+  <si>
+    <t>note2</t>
+  </si>
+  <si>
+    <t>note3</t>
+  </si>
+  <si>
+    <t>note4</t>
+  </si>
+  <si>
+    <t>note5</t>
+  </si>
+  <si>
+    <t>note6</t>
+  </si>
+  <si>
+    <t>note7</t>
+  </si>
+  <si>
+    <t>note8</t>
+  </si>
+  <si>
+    <t>A1A</t>
+  </si>
+  <si>
+    <t>B2B</t>
+  </si>
+  <si>
+    <t>C3C</t>
+  </si>
+  <si>
+    <t>D4D</t>
+  </si>
+  <si>
+    <t>E5E</t>
+  </si>
+  <si>
+    <t>F6F</t>
+  </si>
+  <si>
+    <t>G7G</t>
+  </si>
+  <si>
+    <t>H8H</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Adams</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Jefferson</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Madison</t>
   </si>
 </sst>
 </file>
@@ -671,6 +787,149 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244A02C7-843C-4898-AB5D-5B841F681527}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BCE8E8F-D3A3-40F1-8833-268875482DC5}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382AA366-6878-4799-BCA0-DB885E605AF8}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -730,6 +989,295 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8A8FEA-850B-451C-AE75-2B07EDA36E95}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A57E8C-5E2F-4618-B5C7-203CC6A01E3B}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA287ED-1109-45DA-A1EB-69188F036B86}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -781,7 +1329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF88981-8B50-4F78-9C5B-B8BB3D2D03D2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -847,11 +1395,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598A50A3-9E4E-4CFB-ADBD-32D4519A3413}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -921,7 +1469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C3D5BE-DCDF-4163-B69A-AFB892850139}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -995,7 +1543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52535282-E6A0-43C8-98EF-9D760650685A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1091,7 +1639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6536046B-55FA-4C27-8C41-A3DB3D50526B}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1156,147 +1704,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244A02C7-843C-4898-AB5D-5B841F681527}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BCE8E8F-D3A3-40F1-8833-268875482DC5}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>